<commit_message>
Get new LAs from nomis by making them from the old LAs change the names of some leps to match the new ones use latest LA names for all LAs
</commit_message>
<xml_diff>
--- a/Data/1-3_MCA_lookup/MCA_lookup.xlsx
+++ b/Data/1-3_MCA_lookup/MCA_lookup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/1-3_MCA_lookup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{6D8EFACE-BB29-4A9A-BD23-E31A00C410FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48D98EEC-A5AD-48C3-8A68-E17CBFDF6C92}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{6D8EFACE-BB29-4A9A-BD23-E31A00C410FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B92E128-1FE7-40E1-9FAD-37E4E7AF2BC8}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{590927F8-B368-4BAE-B86A-95B78E7723FB}"/>
   </bookViews>
@@ -786,11 +786,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC651680-CCDF-4E8B-B955-181B170CA34F}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="F32" sqref="F1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>